<commit_message>
Exo Excel Stagiaire Afpa en cours
</commit_message>
<xml_diff>
--- a/Excel/Table Multiplication.xlsx
+++ b/Excel/Table Multiplication.xlsx
@@ -417,7 +417,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.42578125" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -483,7 +483,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:L14" si="0">C$2*$A3</f>
+        <f t="shared" ref="C3:L13" si="0">C$2*$A3</f>
         <v>0</v>
       </c>
       <c r="D3" s="2">
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B13" si="1">B$2*A4</f>
+        <f t="shared" ref="B4:B13" si="1">B$2*$A4</f>
         <v>0</v>
       </c>
       <c r="C4" s="3">

</xml_diff>